<commit_message>
Updated the test synthesis notebook and tables
</commit_message>
<xml_diff>
--- a/tests/validation/test_synthesis/test_synthesis_short.xlsx
+++ b/tests/validation/test_synthesis/test_synthesis_short.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>PDE_model</t>
   </si>
@@ -40,73 +40,151 @@
     <t>Mesh_number_of_elements</t>
   </si>
   <si>
+    <t>Global_name</t>
+  </si>
+  <si>
     <t>Poisson</t>
   </si>
   <si>
     <t>Finite volumes</t>
   </si>
   <si>
-    <t>VF9</t>
-  </si>
-  <si>
-    <t>Non conforming cartesian</t>
+    <t>VF5</t>
+  </si>
+  <si>
+    <t>Regular cubes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexahedra </t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>FV simulation of the 3D Poisson equation</t>
+  </si>
+  <si>
+    <t>Wave system</t>
+  </si>
+  <si>
+    <t>Upwind</t>
+  </si>
+  <si>
+    <t>Unstructured triangles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triangles </t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 104420 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 224 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 40 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 6422 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 25872 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 934 cells</t>
+  </si>
+  <si>
+    <t>Finite elements</t>
+  </si>
+  <si>
+    <t>P1 FE</t>
+  </si>
+  <si>
+    <t>Unstructured 3D triangles</t>
+  </si>
+  <si>
+    <t>FE simulation of the Poisson equation on a sphere</t>
+  </si>
+  <si>
+    <t>Regular squares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quadrangles </t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 2 on 6561 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 2 on 225 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 2 on 49 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 2 on 961 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 2 on 2601 cells</t>
+  </si>
+  <si>
+    <t>Unstructured tetrahedra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tetrahedra </t>
+  </si>
+  <si>
+    <t>Regular tetrahedra</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 750 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 7986 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 55566 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 105456 cells</t>
+  </si>
+  <si>
+    <t>Non conforming cartesian locally refined</t>
   </si>
   <si>
     <t xml:space="preserve">Quadrangles Polygons </t>
   </si>
   <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Wave system</t>
+    <t>FV simulation of the 2D Poisson equation</t>
+  </si>
+  <si>
+    <t>FE simulation of the 2D Poisson equation</t>
   </si>
   <si>
     <t>Pseudo staggered</t>
   </si>
   <si>
-    <t>Regular squares</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quadrangles </t>
-  </si>
-  <si>
-    <t>Finite elements</t>
-  </si>
-  <si>
-    <t>P1 FE</t>
-  </si>
-  <si>
-    <t>Unstructured 3D triangles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Triangles </t>
-  </si>
-  <si>
-    <t>VF27</t>
-  </si>
-  <si>
-    <t>Unstructured tetrahedra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tetrahedra </t>
-  </si>
-  <si>
-    <t>Upwind</t>
-  </si>
-  <si>
-    <t>Unstructured triangles</t>
-  </si>
-  <si>
-    <t>Regular cubes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hexahedra </t>
-  </si>
-  <si>
-    <t>Regular tetrahedra</t>
+    <t>Resolution of the Wave system in dimension 3 on 1331 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 29791 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 9261 cells</t>
+  </si>
+  <si>
+    <t>Non conforming cartesian checkerboard</t>
+  </si>
+  <si>
+    <t>Orange, dark squares. PB with mesh ?</t>
+  </si>
+  <si>
+    <t>FE simulation of the 3D Poisson equation</t>
   </si>
   <si>
     <t xml:space="preserve">Hexahedra Polyhedrons </t>
+  </si>
+  <si>
+    <t>Orange, BC violated. PB with mesh ?</t>
   </si>
 </sst>
 </file>
@@ -123,11 +201,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,15 +232,14 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -460,15 +533,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,2006 +566,2440 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" t="n">
-        <v>163840</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>9261</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="n">
+        <v>68921</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="n">
-        <v>40960</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I4" t="n">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>1331</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E5" t="n">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I5" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>104420</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I6" t="n">
-        <v>2560</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>224</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E7" t="n">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I7" t="n">
-        <v>10240</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>40</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E8" t="n">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I8" t="n">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>6422</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E9" t="n">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I9" t="n">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>25872</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E10" t="n">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I10" t="n">
-        <v>6561</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>934</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E11" t="n">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I11" t="n">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>288</v>
+      </c>
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E12" t="n">
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I12" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>10773</v>
+      </c>
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E13" t="n">
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I13" t="n">
-        <v>2601</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>1124</v>
+      </c>
+      <c r="J13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
         <v>19</v>
       </c>
-      <c r="E14" t="n">
-        <v>2</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" t="s">
-        <v>21</v>
-      </c>
       <c r="H14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I14" t="n">
         <v>2638</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" t="n">
-        <v>2</v>
-      </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" t="s">
-        <v>21</v>
-      </c>
       <c r="H15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I15" t="n">
         <v>4512</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E16" t="n">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I16" t="n">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>6561</v>
+      </c>
+      <c r="J16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E17" t="n">
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I17" t="n">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>225</v>
+      </c>
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E18" t="n">
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I18" t="n">
-        <v>10773</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>49</v>
+      </c>
+      <c r="J18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E19" t="n">
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I19" t="n">
-        <v>40960</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>961</v>
+      </c>
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E20" t="n">
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I20" t="n">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>2601</v>
+      </c>
+      <c r="J20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="H21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I21" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>16834</v>
+      </c>
+      <c r="J21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="H22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I22" t="n">
-        <v>2560</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>28561</v>
+      </c>
+      <c r="J22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="H23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I23" t="n">
-        <v>10240</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>63249</v>
+      </c>
+      <c r="J23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="H24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I24" t="n">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>7629</v>
+      </c>
+      <c r="J24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E25" t="n">
         <v>3</v>
       </c>
       <c r="F25" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="G25" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="H25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I25" t="n">
-        <v>2081</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>270</v>
+      </c>
+      <c r="J25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E26" t="n">
         <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="G26" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="H26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I26" t="n">
         <v>4077</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E27" t="n">
         <v>3</v>
       </c>
       <c r="F27" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="G27" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="H27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I27" t="n">
-        <v>28561</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>2081</v>
+      </c>
+      <c r="J27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E28" t="n">
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="G28" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="H28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I28" t="n">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>750</v>
+      </c>
+      <c r="J28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E29" t="n">
         <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="G29" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="H29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I29" t="n">
-        <v>16834</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>7986</v>
+      </c>
+      <c r="J29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E30" t="n">
         <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="G30" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="H30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I30" t="n">
-        <v>63249</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>55566</v>
+      </c>
+      <c r="J30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E31" t="n">
         <v>3</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="G31" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="H31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I31" t="n">
-        <v>7629</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>105456</v>
+      </c>
+      <c r="J31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E32" t="n">
         <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="H32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I32" t="n">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>2560</v>
+      </c>
+      <c r="J32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E33" t="n">
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="H33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I33" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>40</v>
+      </c>
+      <c r="J33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E34" t="n">
         <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="G34" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="H34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I34" t="n">
-        <v>6561</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>640</v>
+      </c>
+      <c r="J34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E35" t="n">
         <v>2</v>
       </c>
       <c r="F35" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="G35" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="H35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I35" t="n">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>160</v>
+      </c>
+      <c r="J35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E36" t="n">
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="G36" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="H36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I36" t="n">
-        <v>2601</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>10240</v>
+      </c>
+      <c r="J36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E37" t="n">
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="G37" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="H37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I37" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>163840</v>
+      </c>
+      <c r="J37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E38" t="n">
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="G38" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="H38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I38" t="n">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>40960</v>
+      </c>
+      <c r="J38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E39" t="n">
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G39" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I39" t="n">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <v>131</v>
+      </c>
+      <c r="J39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E40" t="n">
         <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G40" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I40" t="n">
-        <v>25872</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>29</v>
+      </c>
+      <c r="J40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E41" t="n">
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G41" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I41" t="n">
-        <v>6422</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+        <v>506</v>
+      </c>
+      <c r="J41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E42" t="n">
         <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G42" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I42" t="n">
-        <v>22801</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>13135</v>
+      </c>
+      <c r="J42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E43" t="n">
         <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G43" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I43" t="n">
-        <v>2601</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>3310</v>
+      </c>
+      <c r="J43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E44" t="n">
         <v>2</v>
       </c>
       <c r="F44" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G44" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="H44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I44" t="n">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>22801</v>
+      </c>
+      <c r="J44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E45" t="n">
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G45" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="H45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I45" t="n">
-        <v>40401</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>2601</v>
+      </c>
+      <c r="J45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F46" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G46" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I46" t="n">
-        <v>1331</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+        <v>121</v>
+      </c>
+      <c r="J46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G47" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I47" t="n">
-        <v>9261</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>40401</v>
+      </c>
+      <c r="J47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="E48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F48" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G48" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I48" t="n">
-        <v>68921</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>6561</v>
+      </c>
+      <c r="J48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F49" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G49" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I49" t="n">
-        <v>9261</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+        <v>2601</v>
+      </c>
+      <c r="J49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G50" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I50" t="n">
-        <v>1331</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>49</v>
+      </c>
+      <c r="J50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G51" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I51" t="n">
-        <v>29791</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>961</v>
+      </c>
+      <c r="J51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E52" t="n">
         <v>2</v>
       </c>
       <c r="F52" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G52" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I52" t="n">
-        <v>3310</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>225</v>
+      </c>
+      <c r="J52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F53" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G53" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I53" t="n">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>1331</v>
+      </c>
+      <c r="J53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C54" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D54" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F54" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G54" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I54" t="n">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>29791</v>
+      </c>
+      <c r="J54" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C55" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E55" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F55" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G55" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I55" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>9261</v>
+      </c>
+      <c r="J55" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E56" t="n">
         <v>2</v>
       </c>
       <c r="F56" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="G56" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="H56" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="I56" t="n">
-        <v>13135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+        <v>2560</v>
+      </c>
+      <c r="J56" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="G57" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="H57" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="I57" t="n">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>40</v>
+      </c>
+      <c r="J57" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D58" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="G58" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="H58" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="I58" t="n">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>640</v>
+      </c>
+      <c r="J58" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D59" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F59" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="G59" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="H59" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="I59" t="n">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+        <v>160</v>
+      </c>
+      <c r="J59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E60" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="G60" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="H60" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="I60" t="n">
-        <v>3372</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>10240</v>
+      </c>
+      <c r="J60" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="G61" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="H61" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="I61" t="n">
-        <v>5956</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+        <v>40960</v>
+      </c>
+      <c r="J61" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="n">
+        <v>2</v>
+      </c>
+      <c r="F62" t="s">
         <v>18</v>
       </c>
-      <c r="D62" t="s">
+      <c r="G62" t="s">
         <v>19</v>
       </c>
-      <c r="E62" t="n">
-        <v>3</v>
-      </c>
-      <c r="F62" t="s">
-        <v>23</v>
-      </c>
-      <c r="G62" t="s">
-        <v>24</v>
-      </c>
       <c r="H62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I62" t="n">
-        <v>1543</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+        <v>25872</v>
+      </c>
+      <c r="J62" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" t="n">
+        <v>2</v>
+      </c>
+      <c r="F63" t="s">
         <v>18</v>
       </c>
-      <c r="D63" t="s">
+      <c r="G63" t="s">
         <v>19</v>
       </c>
-      <c r="E63" t="n">
-        <v>3</v>
-      </c>
-      <c r="F63" t="s">
-        <v>23</v>
-      </c>
-      <c r="G63" t="s">
-        <v>24</v>
-      </c>
       <c r="H63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I63" t="n">
-        <v>12465</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+        <v>40</v>
+      </c>
+      <c r="J63" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D64" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G64" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I64" t="n">
-        <v>7986</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>934</v>
+      </c>
+      <c r="J64" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G65" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I65" t="n">
-        <v>55566</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>224</v>
+      </c>
+      <c r="J65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" s="1" t="n">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E66" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F66" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G66" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I66" t="n">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>6422</v>
+      </c>
+      <c r="J66" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D67" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E67" t="n">
         <v>3</v>
       </c>
       <c r="F67" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G67" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I67" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>12465</v>
+      </c>
+      <c r="J67" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D68" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E68" t="n">
         <v>3</v>
       </c>
       <c r="F68" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G68" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I68" t="n">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>1543</v>
+      </c>
+      <c r="J68" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D69" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E69" t="n">
         <v>3</v>
       </c>
       <c r="F69" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G69" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I69" t="n">
-        <v>2304</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <v>5956</v>
+      </c>
+      <c r="J69" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D70" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E70" t="n">
         <v>3</v>
       </c>
       <c r="F70" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G70" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I70" t="n">
+        <v>74</v>
+      </c>
+      <c r="J70" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" t="s">
+        <v>26</v>
+      </c>
+      <c r="D71" t="s">
+        <v>27</v>
+      </c>
+      <c r="E71" t="n">
+        <v>3</v>
+      </c>
+      <c r="F71" t="s">
+        <v>37</v>
+      </c>
+      <c r="G71" t="s">
+        <v>38</v>
+      </c>
+      <c r="H71" t="s">
+        <v>14</v>
+      </c>
+      <c r="I71" t="n">
+        <v>841</v>
+      </c>
+      <c r="J71" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" t="s">
+        <v>26</v>
+      </c>
+      <c r="D72" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" t="n">
+        <v>3</v>
+      </c>
+      <c r="F72" t="s">
+        <v>37</v>
+      </c>
+      <c r="G72" t="s">
+        <v>38</v>
+      </c>
+      <c r="H72" t="s">
+        <v>14</v>
+      </c>
+      <c r="I72" t="n">
+        <v>3372</v>
+      </c>
+      <c r="J72" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" t="s">
+        <v>27</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3</v>
+      </c>
+      <c r="F73" t="s">
+        <v>37</v>
+      </c>
+      <c r="G73" t="s">
+        <v>38</v>
+      </c>
+      <c r="H73" t="s">
+        <v>14</v>
+      </c>
+      <c r="I73" t="n">
+        <v>508</v>
+      </c>
+      <c r="J73" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" t="n">
+        <v>3</v>
+      </c>
+      <c r="F74" t="s">
+        <v>52</v>
+      </c>
+      <c r="G74" t="s">
+        <v>55</v>
+      </c>
+      <c r="H74" t="s">
+        <v>56</v>
+      </c>
+      <c r="I74" t="n">
+        <v>2304</v>
+      </c>
+      <c r="J74" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" t="n">
+        <v>3</v>
+      </c>
+      <c r="F75" t="s">
+        <v>52</v>
+      </c>
+      <c r="G75" t="s">
+        <v>55</v>
+      </c>
+      <c r="H75" t="s">
+        <v>56</v>
+      </c>
+      <c r="I75" t="n">
         <v>18432</v>
+      </c>
+      <c r="J75" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" t="s">
+        <v>10</v>
+      </c>
+      <c r="D76" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" t="n">
+        <v>3</v>
+      </c>
+      <c r="F76" t="s">
+        <v>52</v>
+      </c>
+      <c r="G76" t="s">
+        <v>55</v>
+      </c>
+      <c r="H76" t="s">
+        <v>56</v>
+      </c>
+      <c r="I76" t="n">
+        <v>288</v>
+      </c>
+      <c r="J76" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" t="n">
+        <v>3</v>
+      </c>
+      <c r="F77" t="s">
+        <v>52</v>
+      </c>
+      <c r="G77" t="s">
+        <v>55</v>
+      </c>
+      <c r="H77" t="s">
+        <v>56</v>
+      </c>
+      <c r="I77" t="n">
+        <v>36</v>
+      </c>
+      <c r="J77" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated csv and xlsx validation test synthesis files
</commit_message>
<xml_diff>
--- a/tests/validation/test_synthesis/test_synthesis_short.xlsx
+++ b/tests/validation/test_synthesis/test_synthesis_short.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>PDE_model</t>
   </si>
@@ -43,148 +43,142 @@
     <t>Global_name</t>
   </si>
   <si>
+    <t>Wave system</t>
+  </si>
+  <si>
+    <t>Finite volumes</t>
+  </si>
+  <si>
+    <t>Upwind</t>
+  </si>
+  <si>
+    <t>Unstructured triangles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triangles </t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 104420 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 224 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 40 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 6422 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 25872 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 934 cells</t>
+  </si>
+  <si>
     <t>Poisson</t>
   </si>
   <si>
-    <t>Finite volumes</t>
+    <t>Finite elements</t>
+  </si>
+  <si>
+    <t>P1 FE</t>
+  </si>
+  <si>
+    <t>Unstructured 3D triangles</t>
+  </si>
+  <si>
+    <t>FE simulation of the Poisson equation on a sphere</t>
+  </si>
+  <si>
+    <t>Regular squares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quadrangles </t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 2 on 6561 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 2 on 225 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 2 on 49 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 2 on 961 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 2 on 2601 cells</t>
+  </si>
+  <si>
+    <t>Regular tetrahedra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tetrahedra </t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 750 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 7986 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 55566 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 105456 cells</t>
   </si>
   <si>
     <t>VF5</t>
   </si>
   <si>
+    <t>Non conforming cartesian locally refined</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quadrangles Polygons </t>
+  </si>
+  <si>
+    <t>FV simulation of the 2D Poisson equation</t>
+  </si>
+  <si>
+    <t>FE simulation of the 2D Poisson equation</t>
+  </si>
+  <si>
     <t>Regular cubes</t>
   </si>
   <si>
     <t xml:space="preserve">Hexahedra </t>
   </si>
   <si>
-    <t>Green</t>
-  </si>
-  <si>
     <t>FV simulation of the 3D Poisson equation</t>
   </si>
   <si>
-    <t>Wave system</t>
-  </si>
-  <si>
-    <t>Upwind</t>
-  </si>
-  <si>
-    <t>Unstructured triangles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Triangles </t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 104420 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 224 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 40 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 6422 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 25872 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 934 cells</t>
-  </si>
-  <si>
-    <t>Finite elements</t>
-  </si>
-  <si>
-    <t>P1 FE</t>
-  </si>
-  <si>
-    <t>Unstructured 3D triangles</t>
-  </si>
-  <si>
-    <t>FE simulation of the Poisson equation on a sphere</t>
-  </si>
-  <si>
-    <t>Regular squares</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quadrangles </t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 2 on 6561 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 2 on 225 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 2 on 49 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 2 on 961 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 2 on 2601 cells</t>
+    <t>Pseudo staggered</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 1331 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 29791 cells</t>
+  </si>
+  <si>
+    <t>Resolution of the Wave system in dimension 3 on 9261 cells</t>
+  </si>
+  <si>
+    <t>Non conforming cartesian checkerboard</t>
+  </si>
+  <si>
+    <t>Orange, dark squares. PB with mesh ?</t>
   </si>
   <si>
     <t>Unstructured tetrahedra</t>
   </si>
   <si>
-    <t xml:space="preserve">Tetrahedra </t>
-  </si>
-  <si>
-    <t>Regular tetrahedra</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 750 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 7986 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 55566 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 105456 cells</t>
-  </si>
-  <si>
-    <t>Non conforming cartesian locally refined</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quadrangles Polygons </t>
-  </si>
-  <si>
-    <t>FV simulation of the 2D Poisson equation</t>
-  </si>
-  <si>
-    <t>FE simulation of the 2D Poisson equation</t>
-  </si>
-  <si>
-    <t>Pseudo staggered</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 1331 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 29791 cells</t>
-  </si>
-  <si>
-    <t>Resolution of the Wave system in dimension 3 on 9261 cells</t>
-  </si>
-  <si>
-    <t>Non conforming cartesian checkerboard</t>
-  </si>
-  <si>
-    <t>Orange, dark squares. PB with mesh ?</t>
-  </si>
-  <si>
     <t>FE simulation of the 3D Poisson equation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hexahedra Polyhedrons </t>
-  </si>
-  <si>
-    <t>Orange, BC violated. PB with mesh ?</t>
   </si>
 </sst>
 </file>
@@ -533,7 +527,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -584,7 +578,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -596,7 +590,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="n">
-        <v>9261</v>
+        <v>104420</v>
       </c>
       <c r="J2" t="s">
         <v>15</v>
@@ -616,7 +610,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -628,10 +622,10 @@
         <v>14</v>
       </c>
       <c r="I3" t="n">
-        <v>68921</v>
+        <v>224</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -648,7 +642,7 @@
         <v>11</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -660,10 +654,10 @@
         <v>14</v>
       </c>
       <c r="I4" t="n">
-        <v>1331</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -671,31 +665,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E5" t="n">
         <v>2</v>
       </c>
       <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="n">
+        <v>6422</v>
+      </c>
+      <c r="J5" t="s">
         <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="n">
-        <v>104420</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -703,31 +697,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="n">
+        <v>25872</v>
+      </c>
+      <c r="J6" t="s">
         <v>19</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" t="n">
-        <v>224</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -735,31 +729,31 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E7" t="n">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
       </c>
       <c r="I7" t="n">
-        <v>40</v>
+        <v>934</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -767,31 +761,31 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E8" t="n">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
       </c>
       <c r="I8" t="n">
-        <v>6422</v>
+        <v>288</v>
       </c>
       <c r="J8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -799,31 +793,31 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E9" t="n">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
       </c>
       <c r="I9" t="n">
-        <v>25872</v>
+        <v>10773</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -831,28 +825,28 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E10" t="n">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
       </c>
       <c r="I10" t="n">
-        <v>934</v>
+        <v>1124</v>
       </c>
       <c r="J10" t="s">
         <v>25</v>
@@ -863,31 +857,31 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E11" t="n">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
         <v>14</v>
       </c>
       <c r="I11" t="n">
-        <v>288</v>
+        <v>2638</v>
       </c>
       <c r="J11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -895,31 +889,31 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E12" t="n">
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
       </c>
       <c r="I12" t="n">
-        <v>10773</v>
+        <v>4512</v>
       </c>
       <c r="J12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -930,28 +924,28 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" t="s">
+      <c r="G13" t="s">
         <v>27</v>
       </c>
-      <c r="E13" t="n">
-        <v>2</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" t="n">
+        <v>6561</v>
+      </c>
+      <c r="J13" t="s">
         <v>28</v>
-      </c>
-      <c r="G13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" t="n">
-        <v>1124</v>
-      </c>
-      <c r="J13" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -962,25 +956,25 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
         <v>26</v>
       </c>
-      <c r="D14" t="s">
+      <c r="G14" t="s">
         <v>27</v>
       </c>
-      <c r="E14" t="n">
-        <v>2</v>
-      </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" t="s">
-        <v>19</v>
-      </c>
       <c r="H14" t="s">
         <v>14</v>
       </c>
       <c r="I14" t="n">
-        <v>2638</v>
+        <v>225</v>
       </c>
       <c r="J14" t="s">
         <v>29</v>
@@ -994,28 +988,28 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s">
+      <c r="G15" t="s">
         <v>27</v>
       </c>
-      <c r="E15" t="n">
-        <v>2</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" t="s">
-        <v>19</v>
-      </c>
       <c r="H15" t="s">
         <v>14</v>
       </c>
       <c r="I15" t="n">
-        <v>4512</v>
+        <v>49</v>
       </c>
       <c r="J15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1023,31 +1017,31 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E16" t="n">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" t="n">
+        <v>961</v>
+      </c>
+      <c r="J16" t="s">
         <v>31</v>
-      </c>
-      <c r="H16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" t="n">
-        <v>6561</v>
-      </c>
-      <c r="J16" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1055,31 +1049,31 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E17" t="n">
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H17" t="s">
         <v>14</v>
       </c>
       <c r="I17" t="n">
-        <v>225</v>
+        <v>2601</v>
       </c>
       <c r="J17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1087,31 +1081,31 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H18" t="s">
         <v>14</v>
       </c>
       <c r="I18" t="n">
-        <v>49</v>
+        <v>750</v>
       </c>
       <c r="J18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1119,31 +1113,31 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H19" t="s">
         <v>14</v>
       </c>
       <c r="I19" t="n">
-        <v>961</v>
+        <v>7986</v>
       </c>
       <c r="J19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1151,31 +1145,31 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H20" t="s">
         <v>14</v>
       </c>
       <c r="I20" t="n">
-        <v>2601</v>
+        <v>55566</v>
       </c>
       <c r="J20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1195,19 +1189,19 @@
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" t="n">
+        <v>105456</v>
+      </c>
+      <c r="J21" t="s">
         <v>38</v>
-      </c>
-      <c r="H21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" t="n">
-        <v>16834</v>
-      </c>
-      <c r="J21" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1215,31 +1209,31 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H22" t="s">
         <v>14</v>
       </c>
       <c r="I22" t="n">
-        <v>28561</v>
+        <v>2560</v>
       </c>
       <c r="J22" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1247,31 +1241,31 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G23" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H23" t="s">
         <v>14</v>
       </c>
       <c r="I23" t="n">
-        <v>63249</v>
+        <v>40</v>
       </c>
       <c r="J23" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1279,31 +1273,31 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G24" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H24" t="s">
         <v>14</v>
       </c>
       <c r="I24" t="n">
-        <v>7629</v>
+        <v>640</v>
       </c>
       <c r="J24" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1311,31 +1305,31 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G25" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H25" t="s">
         <v>14</v>
       </c>
       <c r="I25" t="n">
-        <v>270</v>
+        <v>160</v>
       </c>
       <c r="J25" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1343,31 +1337,31 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G26" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H26" t="s">
         <v>14</v>
       </c>
       <c r="I26" t="n">
-        <v>4077</v>
+        <v>10240</v>
       </c>
       <c r="J26" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1375,31 +1369,31 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G27" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H27" t="s">
         <v>14</v>
       </c>
       <c r="I27" t="n">
-        <v>2081</v>
+        <v>163840</v>
       </c>
       <c r="J27" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1407,31 +1401,31 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G28" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H28" t="s">
         <v>14</v>
       </c>
       <c r="I28" t="n">
-        <v>750</v>
+        <v>40960</v>
       </c>
       <c r="J28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1439,31 +1433,31 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="H29" t="s">
         <v>14</v>
       </c>
       <c r="I29" t="n">
-        <v>7986</v>
+        <v>131</v>
       </c>
       <c r="J29" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1471,31 +1465,31 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="H30" t="s">
         <v>14</v>
       </c>
       <c r="I30" t="n">
-        <v>55566</v>
+        <v>29</v>
       </c>
       <c r="J30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1503,28 +1497,28 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="H31" t="s">
         <v>14</v>
       </c>
       <c r="I31" t="n">
-        <v>105456</v>
+        <v>506</v>
       </c>
       <c r="J31" t="s">
         <v>43</v>
@@ -1535,31 +1529,31 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E32" t="n">
         <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="H32" t="s">
         <v>14</v>
       </c>
       <c r="I32" t="n">
-        <v>2560</v>
+        <v>13135</v>
       </c>
       <c r="J32" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1567,31 +1561,31 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E33" t="n">
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="H33" t="s">
         <v>14</v>
       </c>
       <c r="I33" t="n">
-        <v>40</v>
+        <v>3310</v>
       </c>
       <c r="J33" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1599,16 +1593,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C34" t="s">
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F34" t="s">
         <v>44</v>
@@ -1620,7 +1614,7 @@
         <v>14</v>
       </c>
       <c r="I34" t="n">
-        <v>640</v>
+        <v>9261</v>
       </c>
       <c r="J34" t="s">
         <v>46</v>
@@ -1631,16 +1625,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F35" t="s">
         <v>44</v>
@@ -1652,7 +1646,7 @@
         <v>14</v>
       </c>
       <c r="I35" t="n">
-        <v>160</v>
+        <v>68921</v>
       </c>
       <c r="J35" t="s">
         <v>46</v>
@@ -1663,16 +1657,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E36" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F36" t="s">
         <v>44</v>
@@ -1684,7 +1678,7 @@
         <v>14</v>
       </c>
       <c r="I36" t="n">
-        <v>10240</v>
+        <v>1331</v>
       </c>
       <c r="J36" t="s">
         <v>46</v>
@@ -1695,31 +1689,31 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E37" t="n">
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="G37" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H37" t="s">
         <v>14</v>
       </c>
       <c r="I37" t="n">
-        <v>163840</v>
+        <v>22801</v>
       </c>
       <c r="J37" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1727,31 +1721,31 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C38" t="s">
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E38" t="n">
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="G38" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H38" t="s">
         <v>14</v>
       </c>
       <c r="I38" t="n">
-        <v>40960</v>
+        <v>2601</v>
       </c>
       <c r="J38" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1759,31 +1753,31 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
         <v>26</v>
       </c>
-      <c r="D39" t="s">
+      <c r="G39" t="s">
         <v>27</v>
       </c>
-      <c r="E39" t="n">
-        <v>2</v>
-      </c>
-      <c r="F39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" t="s">
-        <v>19</v>
-      </c>
       <c r="H39" t="s">
         <v>14</v>
       </c>
       <c r="I39" t="n">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="J39" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1791,31 +1785,31 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" t="n">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
         <v>26</v>
       </c>
-      <c r="D40" t="s">
+      <c r="G40" t="s">
         <v>27</v>
       </c>
-      <c r="E40" t="n">
-        <v>2</v>
-      </c>
-      <c r="F40" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" t="s">
-        <v>19</v>
-      </c>
       <c r="H40" t="s">
         <v>14</v>
       </c>
       <c r="I40" t="n">
-        <v>29</v>
+        <v>40401</v>
       </c>
       <c r="J40" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1826,28 +1820,28 @@
         <v>9</v>
       </c>
       <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" t="n">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
         <v>26</v>
       </c>
-      <c r="D41" t="s">
+      <c r="G41" t="s">
         <v>27</v>
       </c>
-      <c r="E41" t="n">
-        <v>2</v>
-      </c>
-      <c r="F41" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" t="s">
-        <v>19</v>
-      </c>
       <c r="H41" t="s">
         <v>14</v>
       </c>
       <c r="I41" t="n">
-        <v>506</v>
+        <v>6561</v>
       </c>
       <c r="J41" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1858,28 +1852,28 @@
         <v>9</v>
       </c>
       <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
         <v>26</v>
       </c>
-      <c r="D42" t="s">
+      <c r="G42" t="s">
         <v>27</v>
       </c>
-      <c r="E42" t="n">
-        <v>2</v>
-      </c>
-      <c r="F42" t="s">
-        <v>18</v>
-      </c>
-      <c r="G42" t="s">
-        <v>19</v>
-      </c>
       <c r="H42" t="s">
         <v>14</v>
       </c>
       <c r="I42" t="n">
-        <v>13135</v>
+        <v>2601</v>
       </c>
       <c r="J42" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1890,28 +1884,28 @@
         <v>9</v>
       </c>
       <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" t="n">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
         <v>26</v>
       </c>
-      <c r="D43" t="s">
+      <c r="G43" t="s">
         <v>27</v>
       </c>
-      <c r="E43" t="n">
-        <v>2</v>
-      </c>
-      <c r="F43" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" t="s">
-        <v>19</v>
-      </c>
       <c r="H43" t="s">
         <v>14</v>
       </c>
       <c r="I43" t="n">
-        <v>3310</v>
+        <v>49</v>
       </c>
       <c r="J43" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1925,25 +1919,25 @@
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="E44" t="n">
         <v>2</v>
       </c>
       <c r="F44" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H44" t="s">
+        <v>14</v>
+      </c>
+      <c r="I44" t="n">
+        <v>961</v>
+      </c>
+      <c r="J44" t="s">
         <v>31</v>
-      </c>
-      <c r="H44" t="s">
-        <v>14</v>
-      </c>
-      <c r="I44" t="n">
-        <v>22801</v>
-      </c>
-      <c r="J44" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1957,25 +1951,25 @@
         <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="E45" t="n">
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G45" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H45" t="s">
         <v>14</v>
       </c>
       <c r="I45" t="n">
-        <v>2601</v>
+        <v>225</v>
       </c>
       <c r="J45" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1992,22 +1986,22 @@
         <v>11</v>
       </c>
       <c r="E46" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F46" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G46" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H46" t="s">
         <v>14</v>
       </c>
       <c r="I46" t="n">
-        <v>121</v>
+        <v>1331</v>
       </c>
       <c r="J46" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2024,22 +2018,22 @@
         <v>11</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F47" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G47" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H47" t="s">
         <v>14</v>
       </c>
       <c r="I47" t="n">
-        <v>40401</v>
+        <v>29791</v>
       </c>
       <c r="J47" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2047,31 +2041,31 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
         <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F48" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G48" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H48" t="s">
         <v>14</v>
       </c>
       <c r="I48" t="n">
-        <v>6561</v>
+        <v>9261</v>
       </c>
       <c r="J48" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2079,31 +2073,31 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
         <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E49" t="n">
         <v>2</v>
       </c>
       <c r="F49" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="G49" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="H49" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="I49" t="n">
-        <v>2601</v>
+        <v>2560</v>
       </c>
       <c r="J49" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2111,31 +2105,31 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C50" t="s">
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E50" t="n">
         <v>2</v>
       </c>
       <c r="F50" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="G50" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="H50" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="I50" t="n">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J50" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2143,31 +2137,31 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C51" t="s">
         <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E51" t="n">
         <v>2</v>
       </c>
       <c r="F51" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="G51" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="H51" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="I51" t="n">
-        <v>961</v>
+        <v>640</v>
       </c>
       <c r="J51" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2175,31 +2169,31 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C52" t="s">
         <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E52" t="n">
         <v>2</v>
       </c>
       <c r="F52" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="G52" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="H52" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="I52" t="n">
-        <v>225</v>
+        <v>160</v>
       </c>
       <c r="J52" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2207,31 +2201,31 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C53" t="s">
         <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="G53" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="H53" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="I53" t="n">
-        <v>1331</v>
+        <v>10240</v>
       </c>
       <c r="J53" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2239,31 +2233,31 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C54" t="s">
         <v>10</v>
       </c>
       <c r="D54" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="G54" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="H54" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="I54" t="n">
-        <v>29791</v>
+        <v>40960</v>
       </c>
       <c r="J54" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2271,16 +2265,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C55" t="s">
         <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="s">
         <v>12</v>
@@ -2292,10 +2286,10 @@
         <v>14</v>
       </c>
       <c r="I55" t="n">
-        <v>9261</v>
+        <v>25872</v>
       </c>
       <c r="J55" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2303,31 +2297,31 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C56" t="s">
         <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E56" t="n">
         <v>2</v>
       </c>
       <c r="F56" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="G56" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="H56" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="I56" t="n">
-        <v>2560</v>
+        <v>40</v>
       </c>
       <c r="J56" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2335,31 +2329,31 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C57" t="s">
         <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E57" t="n">
         <v>2</v>
       </c>
       <c r="F57" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="G57" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="H57" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="I57" t="n">
-        <v>40</v>
+        <v>934</v>
       </c>
       <c r="J57" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2367,31 +2361,31 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C58" t="s">
         <v>10</v>
       </c>
       <c r="D58" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E58" t="n">
         <v>2</v>
       </c>
       <c r="F58" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="G58" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="H58" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="I58" t="n">
-        <v>640</v>
+        <v>224</v>
       </c>
       <c r="J58" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2399,31 +2393,31 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C59" t="s">
         <v>10</v>
       </c>
       <c r="D59" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E59" t="n">
         <v>2</v>
       </c>
       <c r="F59" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="G59" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="H59" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="I59" t="n">
-        <v>160</v>
+        <v>6422</v>
       </c>
       <c r="J59" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2431,31 +2425,31 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F60" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G60" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="H60" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="I60" t="n">
-        <v>10240</v>
+        <v>12465</v>
       </c>
       <c r="J60" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2463,31 +2457,31 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C61" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D61" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F61" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G61" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="H61" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="I61" t="n">
-        <v>40960</v>
+        <v>1543</v>
       </c>
       <c r="J61" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2495,31 +2489,31 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D62" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F62" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G62" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H62" t="s">
         <v>14</v>
       </c>
       <c r="I62" t="n">
-        <v>25872</v>
+        <v>5956</v>
       </c>
       <c r="J62" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2527,31 +2521,31 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D63" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E63" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F63" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G63" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H63" t="s">
         <v>14</v>
       </c>
       <c r="I63" t="n">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="J63" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2559,31 +2553,31 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D64" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F64" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G64" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H64" t="s">
         <v>14</v>
       </c>
       <c r="I64" t="n">
-        <v>934</v>
+        <v>841</v>
       </c>
       <c r="J64" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2591,31 +2585,31 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D65" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F65" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G65" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H65" t="s">
         <v>14</v>
       </c>
       <c r="I65" t="n">
-        <v>224</v>
+        <v>3372</v>
       </c>
       <c r="J65" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2623,31 +2617,31 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D66" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F66" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G66" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H66" t="s">
         <v>14</v>
       </c>
       <c r="I66" t="n">
-        <v>6422</v>
+        <v>508</v>
       </c>
       <c r="J66" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2655,31 +2649,31 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E67" t="n">
         <v>3</v>
       </c>
       <c r="F67" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G67" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H67" t="s">
         <v>14</v>
       </c>
       <c r="I67" t="n">
-        <v>12465</v>
+        <v>16834</v>
       </c>
       <c r="J67" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2687,31 +2681,31 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D68" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E68" t="n">
         <v>3</v>
       </c>
       <c r="F68" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G68" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H68" t="s">
         <v>14</v>
       </c>
       <c r="I68" t="n">
-        <v>1543</v>
+        <v>28561</v>
       </c>
       <c r="J68" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2719,31 +2713,31 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C69" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E69" t="n">
         <v>3</v>
       </c>
       <c r="F69" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G69" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H69" t="s">
         <v>14</v>
       </c>
       <c r="I69" t="n">
-        <v>5956</v>
+        <v>63249</v>
       </c>
       <c r="J69" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2751,31 +2745,31 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C70" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D70" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E70" t="n">
         <v>3</v>
       </c>
       <c r="F70" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G70" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H70" t="s">
         <v>14</v>
       </c>
       <c r="I70" t="n">
-        <v>74</v>
+        <v>7629</v>
       </c>
       <c r="J70" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -2783,31 +2777,31 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C71" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E71" t="n">
         <v>3</v>
       </c>
       <c r="F71" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G71" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H71" t="s">
         <v>14</v>
       </c>
       <c r="I71" t="n">
-        <v>841</v>
+        <v>270</v>
       </c>
       <c r="J71" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -2815,31 +2809,31 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C72" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D72" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E72" t="n">
         <v>3</v>
       </c>
       <c r="F72" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G72" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H72" t="s">
         <v>14</v>
       </c>
       <c r="I72" t="n">
-        <v>3372</v>
+        <v>4077</v>
       </c>
       <c r="J72" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -2847,159 +2841,31 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C73" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E73" t="n">
         <v>3</v>
       </c>
       <c r="F73" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G73" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H73" t="s">
         <v>14</v>
       </c>
       <c r="I73" t="n">
-        <v>508</v>
+        <v>2081</v>
       </c>
       <c r="J73" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="A74" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="B74" t="s">
-        <v>9</v>
-      </c>
-      <c r="C74" t="s">
-        <v>10</v>
-      </c>
-      <c r="D74" t="s">
-        <v>11</v>
-      </c>
-      <c r="E74" t="n">
-        <v>3</v>
-      </c>
-      <c r="F74" t="s">
-        <v>52</v>
-      </c>
-      <c r="G74" t="s">
-        <v>55</v>
-      </c>
-      <c r="H74" t="s">
-        <v>56</v>
-      </c>
-      <c r="I74" t="n">
-        <v>2304</v>
-      </c>
-      <c r="J74" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B75" t="s">
-        <v>9</v>
-      </c>
-      <c r="C75" t="s">
-        <v>10</v>
-      </c>
-      <c r="D75" t="s">
-        <v>11</v>
-      </c>
-      <c r="E75" t="n">
-        <v>3</v>
-      </c>
-      <c r="F75" t="s">
-        <v>52</v>
-      </c>
-      <c r="G75" t="s">
-        <v>55</v>
-      </c>
-      <c r="H75" t="s">
-        <v>56</v>
-      </c>
-      <c r="I75" t="n">
-        <v>18432</v>
-      </c>
-      <c r="J75" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="A76" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" t="s">
-        <v>9</v>
-      </c>
-      <c r="C76" t="s">
-        <v>10</v>
-      </c>
-      <c r="D76" t="s">
-        <v>11</v>
-      </c>
-      <c r="E76" t="n">
-        <v>3</v>
-      </c>
-      <c r="F76" t="s">
-        <v>52</v>
-      </c>
-      <c r="G76" t="s">
-        <v>55</v>
-      </c>
-      <c r="H76" t="s">
-        <v>56</v>
-      </c>
-      <c r="I76" t="n">
-        <v>288</v>
-      </c>
-      <c r="J76" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="A77" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" t="s">
-        <v>10</v>
-      </c>
-      <c r="D77" t="s">
-        <v>11</v>
-      </c>
-      <c r="E77" t="n">
-        <v>3</v>
-      </c>
-      <c r="F77" t="s">
-        <v>52</v>
-      </c>
-      <c r="G77" t="s">
-        <v>55</v>
-      </c>
-      <c r="H77" t="s">
-        <v>56</v>
-      </c>
-      <c r="I77" t="n">
-        <v>36</v>
-      </c>
-      <c r="J77" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>